<commit_message>
Thêm báo cáo, sửa notebook lần cuối
</commit_message>
<xml_diff>
--- a/data/Industry.xlsx
+++ b/data/Industry.xlsx
@@ -2818,7 +2818,7 @@
   <dimension ref="A1:B751"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2888,7 +2888,7 @@
         <v>526</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>